<commit_message>
Fixed missing states on map + rectify data discrepancies for year 2020
</commit_message>
<xml_diff>
--- a/Plotly + Choropleth Map/Dataset_pop/States_pop.xlsx
+++ b/Plotly + Choropleth Map/Dataset_pop/States_pop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb775b60f7163cde/Desktop/Map Viz/Plotly ^M Choropleth Map/Dataset_pop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="311" documentId="8_{6F1BD218-AF57-4C64-B2D3-70F370FAEFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{465C7287-BC2B-49E9-ABAF-61325CFF837B}"/>
+  <xr:revisionPtr revIDLastSave="317" documentId="8_{6F1BD218-AF57-4C64-B2D3-70F370FAEFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78566575-F93C-450E-8FED-917D3A0C40C6}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7810" tabRatio="940" activeTab="1" xr2:uid="{CB78915E-DD85-44B7-BB1E-376C6780AB3F}"/>
+    <workbookView minimized="1" xWindow="-15442" yWindow="-2753" windowWidth="14400" windowHeight="7808" tabRatio="940" xr2:uid="{CB78915E-DD85-44B7-BB1E-376C6780AB3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="16" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="34">
   <si>
     <t>Year</t>
   </si>
@@ -143,6 +143,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Negeri Sembilan</t>
+  </si>
+  <si>
+    <t>Kuala Lumpur</t>
+  </si>
+  <si>
+    <t>Terengganu</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1551,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>N_9</c:v>
+                  <c:v>Negeri Sembilan</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3332,7 +3341,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>T'ganu</c:v>
+                  <c:v>Terengganu</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6185,6 +6194,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6484,9 +6497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746B3F18-905E-441E-8BD1-48B44ECBDFA2}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6508,7 +6521,7 @@
         <v>15</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>17</v>
@@ -6526,7 +6539,7 @@
         <v>21</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="M1" s="11" t="s">
         <v>23</v>
@@ -6535,7 +6548,7 @@
         <v>24</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
@@ -19763,8 +19776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98E1222-AD5B-4542-9DE7-260ADE0FE9D9}">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
@@ -22133,11 +22146,16 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Malaysia's choropleth map & charts for states completed!
</commit_message>
<xml_diff>
--- a/Plotly + Choropleth Map/Dataset_pop/States_pop.xlsx
+++ b/Plotly + Choropleth Map/Dataset_pop/States_pop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb775b60f7163cde/Desktop/Map Viz/Plotly ^M Choropleth Map/Dataset_pop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="317" documentId="8_{6F1BD218-AF57-4C64-B2D3-70F370FAEFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78566575-F93C-450E-8FED-917D3A0C40C6}"/>
+  <xr:revisionPtr revIDLastSave="318" documentId="8_{6F1BD218-AF57-4C64-B2D3-70F370FAEFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{427FB5D2-74D6-46A1-B9E9-88383DC0D256}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-15442" yWindow="-2753" windowWidth="14400" windowHeight="7808" tabRatio="940" xr2:uid="{CB78915E-DD85-44B7-BB1E-376C6780AB3F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="940" xr2:uid="{CB78915E-DD85-44B7-BB1E-376C6780AB3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="16" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="35">
   <si>
     <t>Year</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Terengganu</t>
+  </si>
+  <si>
+    <t>Pulau Pinang</t>
   </si>
 </sst>
 </file>
@@ -2145,7 +2148,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Penang</c:v>
+                  <c:v>Pulau Pinang</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6498,8 +6501,8 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6527,7 +6530,7 @@
         <v>17</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>19</v>

</xml_diff>